<commit_message>
Agrego .gitignore y limpio temporales; versiono generate_json.py e img/
</commit_message>
<xml_diff>
--- a/data/Ejercicios-base.xlsx
+++ b/data/Ejercicios-base.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jehiel Lake\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2025\Proyectos\Gym\buscador-ejercicios\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8818EFF-D7E2-4F84-9DC8-B10AACBE637D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFD472B-9C7F-4087-B45B-C64664A9FEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="284">
   <si>
     <t>ID</t>
   </si>
@@ -869,6 +869,9 @@
   </si>
   <si>
     <t>Principiante</t>
+  </si>
+  <si>
+    <t>EX0058</t>
   </si>
 </sst>
 </file>
@@ -1236,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2937,6 +2940,35 @@
         <v>281</v>
       </c>
     </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>283</v>
+      </c>
+      <c r="B59" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" t="s">
+        <v>122</v>
+      </c>
+      <c r="D59" t="s">
+        <v>176</v>
+      </c>
+      <c r="E59" t="s">
+        <v>192</v>
+      </c>
+      <c r="F59" t="s">
+        <v>216</v>
+      </c>
+      <c r="G59" t="s">
+        <v>273</v>
+      </c>
+      <c r="H59" t="s">
+        <v>274</v>
+      </c>
+      <c r="I59" t="s">
+        <v>281</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>